<commit_message>
Added webinar and classroom training guides
</commit_message>
<xml_diff>
--- a/Modules/Modules.xlsx
+++ b/Modules/Modules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Sync\Red and Bundle\Klanten\ForNAV\Source Code\ForNAV.TrainingModules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Sync\Red and Bundle\Klanten\ForNAV\Source Code\ForNAV.TrainingModules\Modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7655F398-6508-4B32-9253-6E955CC60112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1353E9-D15A-4E61-8C5F-752C6F84DDF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6990" yWindow="2700" windowWidth="24870" windowHeight="15600" xr2:uid="{D270168A-CE25-4ABC-A3BF-FFE5C4C9F529}"/>
+    <workbookView xWindow="39720" yWindow="5775" windowWidth="23775" windowHeight="14355" xr2:uid="{D270168A-CE25-4ABC-A3BF-FFE5C4C9F529}"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Setup</t>
   </si>
@@ -104,24 +104,12 @@
     <t>x</t>
   </si>
   <si>
-    <t>* Basic features under CurrReport</t>
-  </si>
-  <si>
-    <t>* Sections</t>
-  </si>
-  <si>
     <t>Edit your first report</t>
   </si>
   <si>
     <t>Add ForNAV reports to your extensions</t>
   </si>
   <si>
-    <t>* Can Grow</t>
-  </si>
-  <si>
-    <t>Types, placement, repeating</t>
-  </si>
-  <si>
     <t>Related Vid</t>
   </si>
   <si>
@@ -135,9 +123,6 @@
   </si>
   <si>
     <t>* In- en export van layouts en rapporten</t>
-  </si>
-  <si>
-    <t>* Alternating row styles</t>
   </si>
   <si>
     <t>* Create a customer top 10</t>
@@ -218,8 +203,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0FA0F5A6-BCC6-4D96-8856-81F533BDFBD7}" name="Table2" displayName="Table2" ref="A1:E29" totalsRowShown="0">
-  <autoFilter ref="A1:E29" xr:uid="{6AE70C56-E6F2-4171-8CF1-A5EE21541F2E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0FA0F5A6-BCC6-4D96-8856-81F533BDFBD7}" name="Table2" displayName="Table2" ref="A1:E25" totalsRowShown="0">
+  <autoFilter ref="A1:E25" xr:uid="{6AE70C56-E6F2-4171-8CF1-A5EE21541F2E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{58BFF1FD-1F25-445A-9D91-9A59775E8D47}" name="Module"/>
     <tableColumn id="2" xr3:uid="{25E255E6-46EB-41F2-886F-F0283B0EF32E}" name="Web Session"/>
@@ -232,8 +217,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6F184A24-ED18-49CB-B56D-998DE441B474}" name="Table3" displayName="Table3" ref="A31:E36" totalsRowShown="0">
-  <autoFilter ref="A31:E36" xr:uid="{3CE35EB4-4BC0-4AC7-837A-57388DD31F2B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6F184A24-ED18-49CB-B56D-998DE441B474}" name="Table3" displayName="Table3" ref="A27:E32" totalsRowShown="0">
+  <autoFilter ref="A27:E32" xr:uid="{3CE35EB4-4BC0-4AC7-837A-57388DD31F2B}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9ADB18AE-7333-4A78-B706-A0F1C91F3207}" name="Module"/>
     <tableColumn id="2" xr3:uid="{FA1367CE-5CA3-4C7A-860D-F620C35BF0C5}" name="Web Session"/>
@@ -542,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13BC71F3-41AD-4A6F-9554-ADCD6AE34DEF}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +556,7 @@
         <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -607,10 +592,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -624,205 +609,182 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>4</v>
-      </c>
-      <c r="B12">
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
         <v>2</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>9</v>
+      <c r="C11" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="3" t="s">
-        <v>32</v>
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="3" t="s">
-        <v>33</v>
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
         <v>7</v>
-      </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>8</v>
-      </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>10</v>
-      </c>
-      <c r="B22">
-        <v>4</v>
-      </c>
-      <c r="C22" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>11</v>
-      </c>
-      <c r="B24">
-        <v>5</v>
-      </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>30</v>
+      </c>
+      <c r="E24" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>12</v>
-      </c>
-      <c r="B25">
-        <v>5</v>
-      </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>13</v>
-      </c>
-      <c r="B27">
-        <v>6</v>
-      </c>
-      <c r="C27" t="s">
-        <v>16</v>
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>35</v>
-      </c>
-      <c r="E28" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>36</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" t="s">
-        <v>21</v>
-      </c>
-      <c r="E31" t="s">
-        <v>29</v>
+      <c r="C31" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Cust Rep Layout
</commit_message>
<xml_diff>
--- a/Modules/Modules.xlsx
+++ b/Modules/Modules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Sync\Red and Bundle\Klanten\ForNAV\Source Code\ForNAV.TrainingModules\Modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1353E9-D15A-4E61-8C5F-752C6F84DDF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F002FCA-D94C-45D7-BE58-101F199F7636}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39720" yWindow="5775" windowWidth="23775" windowHeight="14355" xr2:uid="{D270168A-CE25-4ABC-A3BF-FFE5C4C9F529}"/>
+    <workbookView xWindow="40410" yWindow="6465" windowWidth="23775" windowHeight="14355" xr2:uid="{D270168A-CE25-4ABC-A3BF-FFE5C4C9F529}"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="2" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>Temp tables</t>
   </si>
   <si>
-    <t>Custom Report Layouts??</t>
-  </si>
-  <si>
     <t>Add data from other tables (Records Collection)</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>* Create Page Ext</t>
+  </si>
+  <si>
+    <t>Custom Report Layouts</t>
   </si>
 </sst>
 </file>
@@ -530,7 +530,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,16 +547,16 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -564,10 +564,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -592,10 +592,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -617,17 +617,17 @@
         <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -660,7 +660,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -671,10 +671,10 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -685,7 +685,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -696,7 +696,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -718,7 +718,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -729,20 +729,20 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -750,21 +750,21 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -784,7 +784,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>